<commit_message>
Poc on using great expectation as data validation rules engine
</commit_message>
<xml_diff>
--- a/poc_expectations.xlsx
+++ b/poc_expectations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KPRO/PycharmProjects/pythonProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KPRO/PycharmProjects/test0/test0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C377F3A5-4455-5D4C-8BD7-3B6DE3DCC71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2CD371-33E0-7C4D-993B-FE0D4A4D9351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="3240" windowWidth="34160" windowHeight="17440" activeTab="2" xr2:uid="{3D7CDF41-D319-394C-8F12-2FDEBAA5A64E}"/>
+    <workbookView xWindow="1680" yWindow="3140" windowWidth="34160" windowHeight="17440" xr2:uid="{3D7CDF41-D319-394C-8F12-2FDEBAA5A64E}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="137">
   <si>
     <t>AccountNumber</t>
   </si>
@@ -145,9 +145,6 @@
     <t>column_exists</t>
   </si>
   <si>
-    <t>column_to_not_be_null</t>
-  </si>
-  <si>
     <t>column_to_be_in_set</t>
   </si>
   <si>
@@ -307,9 +304,6 @@
     <t>Capital must only be one of New York or San Diego</t>
   </si>
   <si>
-    <t>date_column_should_have_format</t>
-  </si>
-  <si>
     <t>DateFormat</t>
   </si>
   <si>
@@ -446,13 +440,25 @@
   </si>
   <si>
     <t>approach to covering complex use cases.</t>
+  </si>
+  <si>
+    <t>column_values_to_not_be_null</t>
+  </si>
+  <si>
+    <t>06012022</t>
+  </si>
+  <si>
+    <t>column_values_to_match_date_format</t>
+  </si>
+  <si>
+    <t>MM-DD-YYYY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -464,6 +470,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -489,10 +501,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1337C836-50CF-9E43-8832-7875BF1F9B99}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -855,8 +868,8 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>6012022</v>
+      <c r="D2" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -878,8 +891,8 @@
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3">
-        <v>6012022</v>
+      <c r="D3" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -895,8 +908,8 @@
       <c r="C4">
         <v>5</v>
       </c>
-      <c r="D4">
-        <v>6012022</v>
+      <c r="D4" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
@@ -912,8 +925,8 @@
       <c r="C5">
         <v>-5</v>
       </c>
-      <c r="D5">
-        <v>6012022</v>
+      <c r="D5" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="G5" t="s">
         <v>24</v>
@@ -929,6 +942,7 @@
       <c r="C6">
         <v>2</v>
       </c>
+      <c r="D6" s="3"/>
       <c r="G6" t="s">
         <v>25</v>
       </c>
@@ -943,8 +957,8 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="D7">
-        <v>6012022</v>
+      <c r="D7" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
@@ -963,8 +977,8 @@
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="D8">
-        <v>6012022</v>
+      <c r="D8" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -986,8 +1000,8 @@
       <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9">
-        <v>6012022</v>
+      <c r="D9" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -1009,8 +1023,8 @@
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10">
-        <v>6012022</v>
+      <c r="D10" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -1032,8 +1046,8 @@
       <c r="C11">
         <v>6</v>
       </c>
-      <c r="D11">
-        <v>6012022</v>
+      <c r="D11" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -1055,8 +1069,8 @@
       <c r="C12">
         <v>7</v>
       </c>
-      <c r="D12">
-        <v>6012022</v>
+      <c r="D12" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -1065,13 +1079,14 @@
         <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I12" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1081,7 +1096,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1089,7 +1104,7 @@
     <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.6640625" bestFit="1" customWidth="1"/>
@@ -1101,57 +1116,57 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
         <v>32</v>
       </c>
       <c r="G1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" t="s">
         <v>45</v>
       </c>
-      <c r="J1" t="s">
-        <v>116</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>46</v>
       </c>
-      <c r="L1" t="s">
-        <v>47</v>
-      </c>
       <c r="M1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -1163,345 +1178,345 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" t="s">
         <v>68</v>
       </c>
-      <c r="L2" t="s">
-        <v>69</v>
-      </c>
       <c r="M2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="J3" t="s">
         <v>0</v>
       </c>
       <c r="K3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" t="s">
         <v>70</v>
-      </c>
-      <c r="L3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J4" t="s">
         <v>0</v>
       </c>
       <c r="K4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L4" t="s">
         <v>72</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>73</v>
-      </c>
-      <c r="M4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="J5" t="s">
         <v>0</v>
       </c>
       <c r="K5" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" t="s">
         <v>75</v>
-      </c>
-      <c r="L5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="I6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J6" t="s">
         <v>0</v>
       </c>
       <c r="K6" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" t="s">
         <v>77</v>
-      </c>
-      <c r="L6" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="I7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J7" t="s">
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="I8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J8" t="s">
         <v>0</v>
       </c>
       <c r="K8" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" t="s">
         <v>79</v>
-      </c>
-      <c r="L8" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J9" t="s">
         <v>0</v>
       </c>
       <c r="K9" t="s">
+        <v>82</v>
+      </c>
+      <c r="L9" t="s">
         <v>83</v>
-      </c>
-      <c r="L9" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J10" t="s">
         <v>0</v>
       </c>
       <c r="K10" t="s">
+        <v>85</v>
+      </c>
+      <c r="L10" t="s">
         <v>86</v>
-      </c>
-      <c r="L10" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
       </c>
       <c r="F11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" t="s">
         <v>88</v>
-      </c>
-      <c r="G11" t="s">
-        <v>90</v>
       </c>
       <c r="J11" t="s">
         <v>3</v>
       </c>
       <c r="K11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J12" t="s">
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J13" t="s">
         <v>19</v>
       </c>
       <c r="K13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2532828E-B9C8-3E42-9A39-4796CE0F53D2}">
           <x14:formula1>
             <xm:f>rules_statics!$C$2:$C$3</xm:f>
@@ -1518,19 +1533,13 @@
           <x14:formula1>
             <xm:f>rules_statics!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>G121 F122:F133</xm:sqref>
+          <xm:sqref>F122:F133</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{23EA9E4D-5FB5-2240-B6C6-FA4AA919E700}">
           <x14:formula1>
             <xm:f>rules_statics!$D$2:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G17:G120</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{585BEA7F-9D4D-2345-84FC-E866962136FC}">
-          <x14:formula1>
-            <xm:f>rules_statics!$D$2:$D$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G16</xm:sqref>
+          <xm:sqref>G2:G180</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{498DA842-8186-C34A-BBF6-55403D43D4C9}">
           <x14:formula1>
@@ -1548,7 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{167C4E90-9B33-564A-9D7B-053B79F041AE}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1561,107 +1570,107 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
         <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
         <v>58</v>
-      </c>
-      <c r="B7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
         <v>60</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1687,7 +1696,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1700,13 +1709,13 @@
         <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1714,55 +1723,59 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>124</v>
+      </c>
+      <c r="D6" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1784,50 +1797,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1835,63 +1848,63 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added data tests and parsing of different date formats
</commit_message>
<xml_diff>
--- a/poc_expectations.xlsx
+++ b/poc_expectations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KPRO/PycharmProjects/test0/test0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\purohitk\dockertest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2CD371-33E0-7C4D-993B-FE0D4A4D9351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F31CD95-CCC0-4DD2-BB0D-A6F2BB6022EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="3140" windowWidth="34160" windowHeight="17440" xr2:uid="{3D7CDF41-D319-394C-8F12-2FDEBAA5A64E}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="26355" windowHeight="11385" xr2:uid="{3D7CDF41-D319-394C-8F12-2FDEBAA5A64E}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -28,12 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="177">
   <si>
     <t>AccountNumber</t>
   </si>
@@ -452,6 +449,126 @@
   </si>
   <si>
     <t>MM-DD-YYYY</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>YYYY</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>MMYYYY</t>
+  </si>
+  <si>
+    <t>YYYYMM</t>
+  </si>
+  <si>
+    <t>MM-YYYY</t>
+  </si>
+  <si>
+    <t>YYYY-MM</t>
+  </si>
+  <si>
+    <t>E-Year</t>
+  </si>
+  <si>
+    <t>stuff</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>1963</t>
+  </si>
+  <si>
+    <t>193</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>E-Month</t>
+  </si>
+  <si>
+    <t>Year must be 4 digits</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>Must be a valid digit month (1-12)</t>
+  </si>
+  <si>
+    <t>032021</t>
+  </si>
+  <si>
+    <t>042021</t>
+  </si>
+  <si>
+    <t>321</t>
+  </si>
+  <si>
+    <t>132021</t>
+  </si>
+  <si>
+    <t>555555</t>
+  </si>
+  <si>
+    <t>062022</t>
+  </si>
+  <si>
+    <t>072022</t>
+  </si>
+  <si>
+    <t>082022</t>
+  </si>
+  <si>
+    <t>092022</t>
+  </si>
+  <si>
+    <t>102022</t>
+  </si>
+  <si>
+    <t>E-MMYYYY</t>
+  </si>
+  <si>
+    <t>Must be a valid MM and YYYY combination</t>
+  </si>
+  <si>
+    <t>1120229</t>
   </si>
 </sst>
 </file>
@@ -820,19 +937,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1337C836-50CF-9E43-8832-7875BF1F9B99}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -858,10 +975,19 @@
         <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -877,11 +1003,20 @@
       <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="L2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -900,8 +1035,17 @@
       <c r="G3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -914,11 +1058,20 @@
       <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="L4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -931,11 +1084,20 @@
       <c r="G5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="L5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -946,11 +1108,20 @@
       <c r="G6" t="s">
         <v>25</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -963,11 +1134,20 @@
       <c r="G7" t="s">
         <v>26</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="L7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -989,8 +1169,17 @@
       <c r="G8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I8" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1009,11 +1198,20 @@
       <c r="G9" t="s">
         <v>28</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1032,11 +1230,20 @@
       <c r="G10" t="s">
         <v>29</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1055,11 +1262,20 @@
       <c r="G11" t="s">
         <v>13</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="L11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1081,7 +1297,16 @@
       <c r="H12" t="s">
         <v>121</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="L12" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1093,28 +1318,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D732DA3-A2D9-414A-83D0-D29B1535FAA9}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.6640625" customWidth="1"/>
-    <col min="11" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="73.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.625" customWidth="1"/>
+    <col min="11" max="11" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="73.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -1155,7 +1380,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -1187,7 +1412,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1216,7 +1441,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -1251,7 +1476,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -1280,7 +1505,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -1312,7 +1537,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -1341,7 +1566,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -1370,7 +1595,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -1402,7 +1627,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1431,7 +1656,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -1460,7 +1685,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -1486,7 +1711,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -1510,13 +1735,103 @@
       </c>
       <c r="L13" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" t="s">
+        <v>138</v>
+      </c>
+      <c r="J14" t="s">
+        <v>137</v>
+      </c>
+      <c r="K14" t="s">
+        <v>144</v>
+      </c>
+      <c r="L14" t="s">
+        <v>161</v>
+      </c>
+      <c r="M14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>149</v>
+      </c>
+      <c r="F15" t="s">
+        <v>135</v>
+      </c>
+      <c r="G15" t="s">
+        <v>139</v>
+      </c>
+      <c r="J15" t="s">
+        <v>149</v>
+      </c>
+      <c r="K15" t="s">
+        <v>160</v>
+      </c>
+      <c r="L15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>140</v>
+      </c>
+      <c r="F16" t="s">
+        <v>135</v>
+      </c>
+      <c r="G16" t="s">
+        <v>140</v>
+      </c>
+      <c r="J16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L16" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2532828E-B9C8-3E42-9A39-4796CE0F53D2}">
           <x14:formula1>
             <xm:f>rules_statics!$C$2:$C$3</xm:f>
@@ -1539,13 +1854,19 @@
           <x14:formula1>
             <xm:f>rules_statics!$D$2:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G180</xm:sqref>
+          <xm:sqref>G78:G180</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{498DA842-8186-C34A-BBF6-55403D43D4C9}">
           <x14:formula1>
             <xm:f>rules_statics!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F121</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8E260293-B2EF-4628-9430-548B30AA70F1}">
+          <x14:formula1>
+            <xm:f>rules_statics!$D$2:$D$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G77</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1561,14 +1882,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -1579,7 +1900,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -1590,7 +1911,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1601,7 +1922,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1612,7 +1933,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -1620,12 +1941,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1633,7 +1954,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -1641,7 +1962,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -1649,7 +1970,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1657,7 +1978,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -1665,7 +1986,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>120</v>
       </c>
@@ -1685,7 +2006,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1693,18 +2014,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B9165B-029C-D843-AE14-7B020DE713A9}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1718,7 +2039,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1732,7 +2053,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -1746,7 +2067,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1757,7 +2078,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>135</v>
       </c>
@@ -1765,12 +2086,42 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>124</v>
       </c>
       <c r="D6" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1787,15 +2138,15 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="177.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -1803,7 +2154,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1811,7 +2162,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -1819,7 +2170,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1827,7 +2178,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1835,7 +2186,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1843,7 +2194,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1851,7 +2202,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -1859,7 +2210,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -1867,7 +2218,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1875,7 +2226,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -1883,7 +2234,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1891,7 +2242,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1899,7 +2250,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>

</xml_diff>